<commit_message>
feat: Gera senha para PDF
</commit_message>
<xml_diff>
--- a/senha/senhas_condominos.xlsx
+++ b/senha/senhas_condominos.xlsx
@@ -22,19 +22,19 @@
     <t>SENHA ARQUIVO</t>
   </si>
   <si>
-    <t>C1705144_A1_Z</t>
-  </si>
-  <si>
-    <t>C1705144_A2_Z</t>
-  </si>
-  <si>
-    <t>C1705145_A1_Z</t>
-  </si>
-  <si>
-    <t>C1705145_A2_Z</t>
-  </si>
-  <si>
-    <t>C1705432_A1_Z</t>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705144_A1_Z.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705144_A2_Z.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705145_A1_Z.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705145_A2_Z.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705432_A1_Z.pdf</t>
   </si>
 </sst>
 </file>
@@ -379,12 +379,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="66" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Remove a senha do PDF
</commit_message>
<xml_diff>
--- a/senha/senhas_condominos.xlsx
+++ b/senha/senhas_condominos.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -22,27 +22,35 @@
     <t>SENHA ARQUIVO</t>
   </si>
   <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705144_A1_Z.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705144_A2_Z.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705145_A1_Z.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705145_A2_Z.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1705432_A1_Z.pdf</t>
+    <t>CAMINHO ARQUIVO</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852538_SPI.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852539_SPI.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852554_SPI.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852789_SPI.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -58,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -66,12 +74,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,64 +435,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
         <v>12345</v>
       </c>
+      <c r="C2" s="2" t="str">
+        <f>RIGHT(A2,16)</f>
+        <v>C1852538_SPI.pdf</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>54321</v>
       </c>
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C5" si="0">RIGHT(A3,16)</f>
+        <v>C1852539_SPI.pdf</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>12354</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>C1852554_SPI.pdf</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>32145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B5" s="1">
         <v>32154</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>C1852789_SPI.pdf</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: Tomada de testes
</commit_message>
<xml_diff>
--- a/senha/senhas_condominos.xlsx
+++ b/senha/senhas_condominos.xlsx
@@ -4,12 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,16 +41,16 @@
     <t>CAMINHO ARQUIVO</t>
   </si>
   <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852538_SPI.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852539_SPI.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852554_SPI.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\C1852789_SPI.pdf</t>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\arquivo01.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\arquivo02.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\arquivo03.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas.Aguiar\Desktop\gerador_senha\pdf\arquivo04.pdf</t>
   </si>
 </sst>
 </file>
@@ -438,14 +454,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -464,50 +480,51 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>12345</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>RIGHT(A2,16)</f>
-        <v>C1852538_SPI.pdf</v>
+        <f>RIGHT(A2,13)</f>
+        <v>arquivo01.pdf</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>54321</v>
+      <c r="B3" s="2">
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f t="shared" ref="C3:C5" si="0">RIGHT(A3,16)</f>
-        <v>C1852539_SPI.pdf</v>
+        <f t="shared" ref="C3:C5" si="0">RIGHT(A3,13)</f>
+        <v>arquivo02.pdf</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <v>32145</v>
+      <c r="B4" s="2">
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C1852554_SPI.pdf</v>
+        <v>arquivo03.pdf</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>32154</v>
+      <c r="B5" s="2">
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C1852789_SPI.pdf</v>
+        <v>arquivo04.pdf</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>